<commit_message>
Product Backlog website checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/Anodiam-Info/LogBook/DailyLogBook.xlsx
+++ b/Offline/BusinessManagement/Information/Anodiam-Info/LogBook/DailyLogBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\Anodiam-Info\LogBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CEACD0-D5AE-4F31-943F-862C48704667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE95A51F-DDF7-4CE2-9763-CAA11FA876E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3624" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-2023" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +97,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -158,9 +170,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,13 +185,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="18" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -200,10 +212,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,7 +480,7 @@
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,152 +491,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="11">
         <v>45282</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11">
         <v>45283</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11">
         <v>45284</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11">
         <v>45285</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11">
         <v>45286</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11">
         <v>45287</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4">
+      <c r="N1" s="11"/>
+      <c r="O1" s="11">
         <v>45288</v>
       </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4">
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11">
         <v>45289</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4">
+      <c r="R1" s="11"/>
+      <c r="S1" s="11">
         <v>45290</v>
       </c>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4">
+      <c r="T1" s="11"/>
+      <c r="U1" s="11">
         <v>45291</v>
       </c>
-      <c r="V1" s="4"/>
+      <c r="V1" s="11"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" s="5" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>0.4548611111111111</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="10">
+        <v>0.75</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="12" t="s">
@@ -655,7 +665,7 @@
       <c r="V4" s="12"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -685,7 +695,7 @@
       <c r="V5" s="12"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">

</xml_diff>